<commit_message>
Add working on learning different quick tests
</commit_message>
<xml_diff>
--- a/AverageLargestAndSmallest.xlsx
+++ b/AverageLargestAndSmallest.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A89BAFE5-9C4C-44D7-BC63-753FCB719A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADBF1E8-5AD6-4245-A93D-9CD68F89BB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{5E61E8B5-A92A-427F-81A5-F199A2E2B26B}"/>
+    <workbookView xWindow="3480" yWindow="3264" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{5E61E8B5-A92A-427F-81A5-F199A2E2B26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$5:$F$49</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Test scores</t>
   </si>
@@ -73,13 +77,34 @@
   </si>
   <si>
     <t>Average of bottom 3 test scores</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>Vinnie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boom </t>
+  </si>
+  <si>
+    <t>Bop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +127,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000099"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,8 +211,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -185,12 +274,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -202,14 +325,124 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="13">
+    <cellStyle name="20% - Accent1 2" xfId="12" xr:uid="{C5A43B21-0583-44F3-80E2-0E0B0ECB4512}"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="20% - Accent3 2" xfId="5" xr:uid="{BE0B3459-5A00-43A6-B99E-797B3E9D2B61}"/>
     <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
+    <cellStyle name="Comment" xfId="9" xr:uid="{C96C014C-B632-424C-B6C1-022BA899AF97}"/>
+    <cellStyle name="Explanatory Text 2" xfId="7" xr:uid="{AD081AC4-28C6-453D-8BA6-DC205B8DD17A}"/>
+    <cellStyle name="Heading 1 2" xfId="6" xr:uid="{C0528F35-3FF5-419D-929A-71BF49311A18}"/>
+    <cellStyle name="Heading 2 2" xfId="11" xr:uid="{E0A932E7-B527-4FC5-BEDC-5FFA10E9FDFD}"/>
+    <cellStyle name="Heading 3 2" xfId="10" xr:uid="{9CB8A718-46F7-47DB-AAD2-F9ED9DF0EBE7}"/>
+    <cellStyle name="Input 2" xfId="8" xr:uid="{009B3025-FB63-4006-8F4E-E8BDFF786FBF}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{75D61046-26CB-4C34-9BA2-628AE8A96797}"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{556584F7-CB5C-4060-98A0-7F0C40C180E0}">
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="totalRow" dxfId="7"/>
+      <tableStyleElement type="firstColumn" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+    </tableStyle>
+    <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{A84C599E-ECC0-4F69-AC10-E52676E842A0}">
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="totalRow" dxfId="3"/>
+      <tableStyleElement type="firstColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -448,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD7CEC0-B676-44B9-85F2-5ADE0A184C48}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,4 +787,58 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A763CC9F-12EB-424E-B514-446EF6674F21}">
+  <dimension ref="B3:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:D5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Mark"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add working on another test
</commit_message>
<xml_diff>
--- a/AverageLargestAndSmallest.xlsx
+++ b/AverageLargestAndSmallest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADBF1E8-5AD6-4245-A93D-9CD68F89BB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A730CDE-492D-4E8F-844D-710BCF4FA567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="3264" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{5E61E8B5-A92A-427F-81A5-F199A2E2B26B}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>Test scores</t>
   </si>
@@ -340,7 +340,57 @@
     <cellStyle name="Normal 2" xfId="4" xr:uid="{75D61046-26CB-4C34-9BA2-628AE8A96797}"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -431,16 +481,16 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{556584F7-CB5C-4060-98A0-7F0C40C180E0}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="totalRow" dxfId="7"/>
-      <tableStyleElement type="firstColumn" dxfId="6"/>
-      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{A84C599E-ECC0-4F69-AC10-E52676E842A0}">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="totalRow" dxfId="3"/>
-      <tableStyleElement type="firstColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstColumn" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -791,10 +841,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A763CC9F-12EB-424E-B514-446EF6674F21}">
-  <dimension ref="B3:D5"/>
+  <dimension ref="B3:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.59765625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,10 +882,86 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Mark"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8:D10">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="im">
+      <formula>NOT(ISERROR(SEARCH("im",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:D15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>"marc"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>